<commit_message>
Updated tests and ran pytests successfully
</commit_message>
<xml_diff>
--- a/tests/testdata/test_all_criteria.xlsx
+++ b/tests/testdata/test_all_criteria.xlsx
@@ -9,9 +9,9 @@
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="Criteria Failing, Air Speed 0.1" sheetId="2" r:id="rId2"/>
-    <sheet name="Criterion 2, Air Speed 0.1" sheetId="3" r:id="rId3"/>
-    <sheet name="Criterion 1, Air Speed 0.1" sheetId="4" r:id="rId4"/>
-    <sheet name="Criterion 3, Air Speed 0.1" sheetId="5" r:id="rId5"/>
+    <sheet name="Criterion 1, Air Speed 0.1" sheetId="3" r:id="rId3"/>
+    <sheet name="Criterion 3, Air Speed 0.1" sheetId="4" r:id="rId4"/>
+    <sheet name="Criterion 2, Air Speed 0.1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -20,18 +20,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="58">
   <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
     <t>JobNo</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -44,25 +44,25 @@
     <t>3</t>
   </si>
   <si>
+    <t>jovyan</t>
+  </si>
+  <si>
+    <t>Criteria Failing, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 1, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 3, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 2, Air Speed 0.1</t>
+  </si>
+  <si>
     <t>/c/e</t>
   </si>
   <si>
-    <t>20220228</t>
-  </si>
-  <si>
-    <t>jovyan</t>
-  </si>
-  <si>
-    <t>Criteria Failing, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 2, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 1, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 3, Air Speed 0.1</t>
+    <t>20220302</t>
   </si>
   <si>
     <t>index</t>
@@ -176,22 +176,22 @@
     <t>1 &amp; 2</t>
   </si>
   <si>
+    <t>Criterion 1 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 1 Relative Change (%)</t>
+  </si>
+  <si>
+    <t>Criterion 3 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 3 Relative Change (%)</t>
+  </si>
+  <si>
     <t>Criterion 2 Absolute Change</t>
   </si>
   <si>
     <t>Criterion 2 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>Criterion 1 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 1 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>Criterion 3 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 3 Relative Change (%)</t>
   </si>
 </sst>
 </file>
@@ -375,10 +375,10 @@
   <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="JobNo"/>
-    <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="Author"/>
-    <tableColumn id="5" name="sheet_name"/>
+    <tableColumn id="2" name="Author"/>
+    <tableColumn id="3" name="sheet_name"/>
+    <tableColumn id="4" name="JobNo"/>
+    <tableColumn id="5" name="Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -406,8 +406,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 2 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 2 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -421,8 +421,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -436,8 +436,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 2 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 2 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -771,10 +771,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -785,13 +785,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -802,13 +802,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -819,10 +819,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -1359,10 +1359,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1379,16 +1379,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>7.8</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>7.9</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.1000000000000005</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1.282051282051289</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1399,16 +1399,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>8.1</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-0.09999999999999964</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-1.234567901234563</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1487,16 +1487,16 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>10.6</v>
       </c>
       <c r="D9">
-        <v>26</v>
+        <v>10.6</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1507,10 +1507,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1527,10 +1527,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>31</v>
+        <v>11.6</v>
       </c>
       <c r="D11">
-        <v>31</v>
+        <v>11.6</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1547,16 +1547,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>29</v>
+        <v>26.3</v>
       </c>
       <c r="D12">
-        <v>29</v>
+        <v>26.4</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.09999999999999787</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.3802281368821211</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1584,10 +1584,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1604,10 +1604,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1641,10 +1641,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>29</v>
+        <v>12.9</v>
       </c>
       <c r="D17">
-        <v>29</v>
+        <v>12.9</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1661,10 +1661,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>28.3</v>
       </c>
       <c r="D18">
-        <v>30</v>
+        <v>28.3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1681,16 +1681,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>33</v>
+        <v>13.4</v>
       </c>
       <c r="D19">
-        <v>33</v>
+        <v>13.5</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.09999999999999964</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.7462686567164152</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1701,16 +1701,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>30</v>
+        <v>28.6</v>
       </c>
       <c r="D20">
-        <v>30</v>
+        <v>28.5</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>-0.1000000000000014</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>-0.3496503496503546</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1721,15 +1721,12 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -1741,10 +1738,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1761,10 +1758,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>0.4</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>0.4</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1781,15 +1778,12 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -1801,10 +1795,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>18</v>
+        <v>5.6</v>
       </c>
       <c r="D25">
-        <v>18</v>
+        <v>5.6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1821,16 +1815,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="D26">
-        <v>22</v>
+        <v>17.8</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.5649717514124375</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1841,10 +1835,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>5.2</v>
       </c>
       <c r="D27">
-        <v>21</v>
+        <v>5.2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1861,10 +1855,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="D28">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1990,10 +1984,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2010,16 +2004,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>7.8</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>7.9</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>0.1000000000000005</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1.282051282051289</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2030,16 +2024,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>8.1</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>-0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>-1.234567901234563</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2118,10 +2112,10 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2138,10 +2132,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2158,10 +2152,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2178,16 +2172,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>26.3</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>26.4</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>0.09999999999999787</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.3802281368821211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2215,10 +2209,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2235,10 +2229,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2272,10 +2266,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2292,10 +2286,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2312,16 +2306,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>13.4</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>13.5</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.7462686567164152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2332,16 +2326,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>28.6</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>28.5</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>-0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>-0.3496503496503546</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2352,12 +2346,15 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -2369,10 +2366,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2389,10 +2386,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2409,12 +2406,15 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -2426,10 +2426,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2446,16 +2446,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>17.8</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0.5649717514124375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2466,10 +2466,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -2486,10 +2486,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2615,10 +2615,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2635,10 +2635,10 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2655,10 +2655,10 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2743,16 +2743,16 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2763,10 +2763,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2783,10 +2783,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2803,10 +2803,10 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2840,10 +2840,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2860,10 +2860,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2897,10 +2897,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2917,10 +2917,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2937,10 +2937,10 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2957,10 +2957,10 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2997,10 +2997,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -3017,10 +3017,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -3057,10 +3057,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -3077,10 +3077,10 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -3097,10 +3097,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -3117,10 +3117,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E28">
         <v>0</v>

</xml_diff>

<commit_message>
All scripts now working successfully
</commit_message>
<xml_diff>
--- a/tests/testdata/test_all_criteria.xlsx
+++ b/tests/testdata/test_all_criteria.xlsx
@@ -9,9 +9,9 @@
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="Criteria Failing, Air Speed 0.1" sheetId="2" r:id="rId2"/>
-    <sheet name="Criterion 1, Air Speed 0.1" sheetId="3" r:id="rId3"/>
-    <sheet name="Criterion 3, Air Speed 0.1" sheetId="4" r:id="rId4"/>
-    <sheet name="Criterion 2, Air Speed 0.1" sheetId="5" r:id="rId5"/>
+    <sheet name="Criterion 3, Air Speed 0.1" sheetId="3" r:id="rId3"/>
+    <sheet name="Criterion 2, Air Speed 0.1" sheetId="4" r:id="rId4"/>
+    <sheet name="Criterion 1, Air Speed 0.1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -20,18 +20,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="58">
   <si>
+    <t>JobNo</t>
+  </si>
+  <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Author</t>
   </si>
   <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
-    <t>JobNo</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -44,27 +44,27 @@
     <t>3</t>
   </si>
   <si>
+    <t>/c/e</t>
+  </si>
+  <si>
+    <t>Criteria Failing, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 3, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 2, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 1, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>20220303</t>
+  </si>
+  <si>
     <t>jovyan</t>
   </si>
   <si>
-    <t>Criteria Failing, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 1, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 3, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 2, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>/c/e</t>
-  </si>
-  <si>
-    <t>20220302</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -176,22 +176,22 @@
     <t>1 &amp; 2</t>
   </si>
   <si>
+    <t>Criterion 3 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 3 Relative Change (%)</t>
+  </si>
+  <si>
+    <t>Criterion 2 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 2 Relative Change (%)</t>
+  </si>
+  <si>
     <t>Criterion 1 Absolute Change</t>
   </si>
   <si>
     <t>Criterion 1 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>Criterion 3 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 3 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>Criterion 2 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 2 Relative Change (%)</t>
   </si>
 </sst>
 </file>
@@ -375,10 +375,10 @@
   <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="Author"/>
+    <tableColumn id="2" name="JobNo"/>
     <tableColumn id="3" name="sheet_name"/>
-    <tableColumn id="4" name="JobNo"/>
-    <tableColumn id="5" name="Date"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -406,8 +406,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -421,8 +421,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 2 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 2 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -436,8 +436,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 2 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 2 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1359,10 +1359,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1379,16 +1379,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>7.8</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>7.9</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>0.1000000000000005</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1.282051282051289</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1399,16 +1399,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>8.1</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>-0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>-1.234567901234563</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1487,10 +1487,10 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1507,10 +1507,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1527,10 +1527,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1547,16 +1547,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>26.3</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>26.4</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>0.09999999999999787</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.3802281368821211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1584,10 +1584,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1604,10 +1604,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1641,10 +1641,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1661,10 +1661,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1681,16 +1681,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>13.4</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>13.5</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.7462686567164152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1701,16 +1701,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>28.6</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>28.5</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>-0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>-0.3496503496503546</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1721,12 +1721,15 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -1738,10 +1741,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1758,10 +1761,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1778,12 +1781,15 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -1795,10 +1801,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1815,16 +1821,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>17.8</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0.5649717514124375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1835,10 +1841,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1855,10 +1861,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1984,10 +1990,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2004,10 +2010,10 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2024,10 +2030,10 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2112,16 +2118,16 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2132,10 +2138,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2152,10 +2158,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2172,10 +2178,10 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2209,10 +2215,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2229,10 +2235,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2266,10 +2272,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2286,10 +2292,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2306,10 +2312,10 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2326,10 +2332,10 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2366,10 +2372,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2386,10 +2392,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2426,10 +2432,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2446,10 +2452,10 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -2466,10 +2472,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -2486,10 +2492,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2615,10 +2621,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2635,16 +2641,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>7.8</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>7.9</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.1000000000000005</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1.282051282051289</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2655,16 +2661,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>8.1</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-0.09999999999999964</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-1.234567901234563</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2743,16 +2749,16 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>10.6</v>
       </c>
       <c r="D9">
-        <v>26</v>
+        <v>10.6</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2763,10 +2769,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2783,10 +2789,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>31</v>
+        <v>11.6</v>
       </c>
       <c r="D11">
-        <v>31</v>
+        <v>11.6</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2803,16 +2809,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>29</v>
+        <v>26.3</v>
       </c>
       <c r="D12">
-        <v>29</v>
+        <v>26.4</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.09999999999999787</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.3802281368821211</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2840,10 +2846,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2860,10 +2866,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2897,10 +2903,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>29</v>
+        <v>12.9</v>
       </c>
       <c r="D17">
-        <v>29</v>
+        <v>12.9</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2917,10 +2923,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>28.3</v>
       </c>
       <c r="D18">
-        <v>30</v>
+        <v>28.3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2937,16 +2943,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>33</v>
+        <v>13.4</v>
       </c>
       <c r="D19">
-        <v>33</v>
+        <v>13.5</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.09999999999999964</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.7462686567164152</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2957,16 +2963,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>30</v>
+        <v>28.6</v>
       </c>
       <c r="D20">
-        <v>30</v>
+        <v>28.5</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>-0.1000000000000014</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>-0.3496503496503546</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2977,15 +2983,12 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -2997,10 +3000,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -3017,10 +3020,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>0.4</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>0.4</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -3037,15 +3040,12 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -3057,10 +3057,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>18</v>
+        <v>5.6</v>
       </c>
       <c r="D25">
-        <v>18</v>
+        <v>5.6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -3077,16 +3077,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="D26">
-        <v>22</v>
+        <v>17.8</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.5649717514124375</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3097,10 +3097,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>5.2</v>
       </c>
       <c r="D27">
-        <v>21</v>
+        <v>5.2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -3117,10 +3117,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="D28">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="E28">
         <v>0</v>

</xml_diff>

<commit_message>
pytest ran. Commented out operative temp test as API call not working any more to obtain it
</commit_message>
<xml_diff>
--- a/tests/testdata/test_all_criteria.xlsx
+++ b/tests/testdata/test_all_criteria.xlsx
@@ -9,9 +9,9 @@
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="Criteria Failing, Air Speed 0.1" sheetId="2" r:id="rId2"/>
-    <sheet name="Criterion 3, Air Speed 0.1" sheetId="3" r:id="rId3"/>
-    <sheet name="Criterion 2, Air Speed 0.1" sheetId="4" r:id="rId4"/>
-    <sheet name="Criterion 1, Air Speed 0.1" sheetId="5" r:id="rId5"/>
+    <sheet name="Criterion 2, Air Speed 0.1" sheetId="3" r:id="rId3"/>
+    <sheet name="Criterion 1, Air Speed 0.1" sheetId="4" r:id="rId4"/>
+    <sheet name="Criterion 3, Air Speed 0.1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -50,15 +50,15 @@
     <t>Criteria Failing, Air Speed 0.1</t>
   </si>
   <si>
+    <t>Criterion 2, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 1, Air Speed 0.1</t>
+  </si>
+  <si>
     <t>Criterion 3, Air Speed 0.1</t>
   </si>
   <si>
-    <t>Criterion 2, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 1, Air Speed 0.1</t>
-  </si>
-  <si>
     <t>20220303</t>
   </si>
   <si>
@@ -176,22 +176,22 @@
     <t>1 &amp; 2</t>
   </si>
   <si>
+    <t>Criterion 2 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 2 Relative Change (%)</t>
+  </si>
+  <si>
+    <t>Criterion 1 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 1 Relative Change (%)</t>
+  </si>
+  <si>
     <t>Criterion 3 Absolute Change</t>
   </si>
   <si>
     <t>Criterion 3 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>Criterion 2 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 2 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>Criterion 1 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 1 Relative Change (%)</t>
   </si>
 </sst>
 </file>
@@ -406,8 +406,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 2 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 2 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -421,8 +421,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 2 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 2 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -436,8 +436,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1359,10 +1359,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1379,10 +1379,10 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1399,10 +1399,10 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1487,16 +1487,16 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1507,10 +1507,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1527,10 +1527,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1547,10 +1547,10 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1584,10 +1584,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1604,10 +1604,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1641,10 +1641,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1661,10 +1661,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1681,10 +1681,10 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1701,10 +1701,10 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1741,10 +1741,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1761,10 +1761,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1801,10 +1801,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1821,10 +1821,10 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1841,10 +1841,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1861,10 +1861,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1990,10 +1990,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2010,16 +2010,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>7.8</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>7.9</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.1000000000000005</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1.282051282051289</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2030,16 +2030,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>8.1</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-0.09999999999999964</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-1.234567901234563</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2118,16 +2118,16 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>10.6</v>
       </c>
       <c r="D9">
-        <v>26</v>
+        <v>10.6</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2138,10 +2138,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2158,10 +2158,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>31</v>
+        <v>11.6</v>
       </c>
       <c r="D11">
-        <v>31</v>
+        <v>11.6</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2178,16 +2178,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>29</v>
+        <v>26.3</v>
       </c>
       <c r="D12">
-        <v>29</v>
+        <v>26.4</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.09999999999999787</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.3802281368821211</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2215,10 +2215,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2235,10 +2235,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2272,10 +2272,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>29</v>
+        <v>12.9</v>
       </c>
       <c r="D17">
-        <v>29</v>
+        <v>12.9</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2292,10 +2292,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>28.3</v>
       </c>
       <c r="D18">
-        <v>30</v>
+        <v>28.3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2312,16 +2312,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>33</v>
+        <v>13.4</v>
       </c>
       <c r="D19">
-        <v>33</v>
+        <v>13.5</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.09999999999999964</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.7462686567164152</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2332,16 +2332,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>30</v>
+        <v>28.6</v>
       </c>
       <c r="D20">
-        <v>30</v>
+        <v>28.5</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>-0.1000000000000014</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>-0.3496503496503546</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2352,15 +2352,12 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -2372,10 +2369,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2392,10 +2389,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>0.4</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>0.4</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2412,15 +2409,12 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -2432,10 +2426,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>18</v>
+        <v>5.6</v>
       </c>
       <c r="D25">
-        <v>18</v>
+        <v>5.6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2452,16 +2446,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="D26">
-        <v>22</v>
+        <v>17.8</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.5649717514124375</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2472,10 +2466,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>5.2</v>
       </c>
       <c r="D27">
-        <v>21</v>
+        <v>5.2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -2492,10 +2486,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="D28">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2621,10 +2615,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2641,16 +2635,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>7.8</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>7.9</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>0.1000000000000005</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1.282051282051289</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2661,16 +2655,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>8.1</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>-0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>-1.234567901234563</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2749,10 +2743,10 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2769,10 +2763,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2789,10 +2783,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2809,16 +2803,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>26.3</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>26.4</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>0.09999999999999787</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.3802281368821211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2846,10 +2840,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2866,10 +2860,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2903,10 +2897,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2923,10 +2917,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2943,16 +2937,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>13.4</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>13.5</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.7462686567164152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2963,16 +2957,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>28.6</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>28.5</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>-0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>-0.3496503496503546</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2983,12 +2977,15 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -3000,10 +2997,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -3020,10 +3017,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -3040,12 +3037,15 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -3057,10 +3057,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -3077,16 +3077,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>17.8</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0.5649717514124375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3097,10 +3097,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -3117,10 +3117,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed operative temperature pytest
</commit_message>
<xml_diff>
--- a/tests/testdata/test_all_criteria.xlsx
+++ b/tests/testdata/test_all_criteria.xlsx
@@ -10,8 +10,8 @@
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="Criteria Failing, Air Speed 0.1" sheetId="2" r:id="rId2"/>
     <sheet name="Criterion 2, Air Speed 0.1" sheetId="3" r:id="rId3"/>
-    <sheet name="Criterion 1, Air Speed 0.1" sheetId="4" r:id="rId4"/>
-    <sheet name="Criterion 3, Air Speed 0.1" sheetId="5" r:id="rId5"/>
+    <sheet name="Criterion 3, Air Speed 0.1" sheetId="4" r:id="rId4"/>
+    <sheet name="Criterion 1, Air Speed 0.1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -53,13 +53,13 @@
     <t>Criterion 2, Air Speed 0.1</t>
   </si>
   <si>
+    <t>Criterion 3, Air Speed 0.1</t>
+  </si>
+  <si>
     <t>Criterion 1, Air Speed 0.1</t>
   </si>
   <si>
-    <t>Criterion 3, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>20220303</t>
+    <t>20220304</t>
   </si>
   <si>
     <t>jovyan</t>
@@ -182,16 +182,16 @@
     <t>Criterion 2 Relative Change (%)</t>
   </si>
   <si>
+    <t>Criterion 3 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 3 Relative Change (%)</t>
+  </si>
+  <si>
     <t>Criterion 1 Absolute Change</t>
   </si>
   <si>
     <t>Criterion 1 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>Criterion 3 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 3 Relative Change (%)</t>
   </si>
 </sst>
 </file>
@@ -421,8 +421,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -436,8 +436,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1990,10 +1990,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2010,16 +2010,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>7.8</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>7.9</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>0.1000000000000005</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1.282051282051289</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2030,16 +2030,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>8.1</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>-0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>-1.234567901234563</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2118,10 +2118,10 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2138,10 +2138,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2158,10 +2158,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2178,16 +2178,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>26.3</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>26.4</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>0.09999999999999787</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.3802281368821211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2215,10 +2215,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2235,10 +2235,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2272,10 +2272,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2292,10 +2292,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2312,16 +2312,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>13.4</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>13.5</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.7462686567164152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2332,16 +2332,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>28.6</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>28.5</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>-0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>-0.3496503496503546</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2352,12 +2352,15 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -2369,10 +2372,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2389,10 +2392,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2409,12 +2412,15 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -2426,10 +2432,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2446,16 +2452,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>17.8</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0.5649717514124375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2466,10 +2472,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -2486,10 +2492,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2615,10 +2621,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2635,16 +2641,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>7.8</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.1000000000000005</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1.282051282051289</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2655,16 +2661,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>8.1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-0.09999999999999964</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-1.234567901234563</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2743,10 +2749,10 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>10.6</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>10.6</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2763,10 +2769,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2783,10 +2789,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>11.6</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>11.6</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2803,16 +2809,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>26.3</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>26.4</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.09999999999999787</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.3802281368821211</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2840,10 +2846,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2860,10 +2866,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2897,10 +2903,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>12.9</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>12.9</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2917,10 +2923,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>28.3</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>28.3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2937,16 +2943,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>13.4</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>13.5</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.09999999999999964</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.7462686567164152</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2957,16 +2963,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>28.6</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>28.5</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>-0.1000000000000014</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>-0.3496503496503546</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2977,15 +2983,12 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -2997,10 +3000,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -3017,10 +3020,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -3037,15 +3040,12 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -3057,10 +3057,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -3077,16 +3077,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>17.8</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.5649717514124375</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3097,10 +3097,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>5.2</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>5.2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -3117,10 +3117,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="E28">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed pytests and ran successfully
</commit_message>
<xml_diff>
--- a/tests/testdata/test_all_criteria.xlsx
+++ b/tests/testdata/test_all_criteria.xlsx
@@ -9,29 +9,29 @@
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="Criteria Failing, Air Speed 0.1" sheetId="2" r:id="rId2"/>
-    <sheet name="Criterion 2, Air Speed 0.1" sheetId="3" r:id="rId3"/>
-    <sheet name="Criterion 1, Air Speed 0.1" sheetId="4" r:id="rId4"/>
-    <sheet name="Criterion 3, Air Speed 0.1" sheetId="5" r:id="rId5"/>
+    <sheet name="Criterion 3, Air Speed 0.1" sheetId="3" r:id="rId3"/>
+    <sheet name="Criterion 2, Air Speed 0.1" sheetId="4" r:id="rId4"/>
+    <sheet name="Criterion 1, Air Speed 0.1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="59">
   <si>
     <t>JobNo</t>
   </si>
   <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>sheet_name</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -47,24 +47,24 @@
     <t>/c/e</t>
   </si>
   <si>
+    <t>jovyan</t>
+  </si>
+  <si>
+    <t>20220308</t>
+  </si>
+  <si>
     <t>Criteria Failing, Air Speed 0.1</t>
   </si>
   <si>
+    <t>Criterion 3, Air Speed 0.1</t>
+  </si>
+  <si>
     <t>Criterion 2, Air Speed 0.1</t>
   </si>
   <si>
     <t>Criterion 1, Air Speed 0.1</t>
   </si>
   <si>
-    <t>Criterion 3, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>20220303</t>
-  </si>
-  <si>
-    <t>jovyan</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -176,6 +176,12 @@
     <t>1 &amp; 2</t>
   </si>
   <si>
+    <t>Criterion 3 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 3 Relative Change (%)</t>
+  </si>
+  <si>
     <t>Criterion 2 Absolute Change</t>
   </si>
   <si>
@@ -188,10 +194,7 @@
     <t>Criterion 1 Relative Change (%)</t>
   </si>
   <si>
-    <t>Criterion 3 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 3 Relative Change (%)</t>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -376,9 +379,9 @@
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="JobNo"/>
-    <tableColumn id="3" name="sheet_name"/>
+    <tableColumn id="3" name="Author"/>
     <tableColumn id="4" name="Date"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="5" name="sheet_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -406,8 +409,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 2 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 2 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -421,8 +424,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 2 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 2 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -436,8 +439,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -771,10 +774,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -785,13 +788,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -802,13 +805,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -819,10 +822,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -1359,10 +1362,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1379,10 +1382,10 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1399,10 +1402,10 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1487,16 +1490,16 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1507,10 +1510,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1527,10 +1530,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1547,10 +1550,10 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1584,10 +1587,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1604,10 +1607,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1641,10 +1644,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1661,10 +1664,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1681,10 +1684,10 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1701,10 +1704,10 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1741,10 +1744,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1761,10 +1764,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1801,10 +1804,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1821,10 +1824,10 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1841,10 +1844,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1861,10 +1864,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1990,10 +1993,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2.5</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>2.5</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2010,16 +2013,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>7.8</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>7.9</v>
+        <v>14</v>
       </c>
       <c r="E3">
-        <v>0.1000000000000005</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1.282051282051289</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2030,16 +2033,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>8.1</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E4">
-        <v>-0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>-1.234567901234563</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2118,16 +2121,16 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>10.6</v>
+        <v>25</v>
       </c>
       <c r="D9">
-        <v>10.6</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2138,10 +2141,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2158,10 +2161,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>11.6</v>
+        <v>31</v>
       </c>
       <c r="D11">
-        <v>11.6</v>
+        <v>31</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2178,16 +2181,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>26.3</v>
+        <v>29</v>
       </c>
       <c r="D12">
-        <v>26.4</v>
+        <v>29</v>
       </c>
       <c r="E12">
-        <v>0.09999999999999787</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.3802281368821211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2215,10 +2218,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>0.6</v>
+        <v>5</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2235,10 +2238,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2272,10 +2275,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>12.9</v>
+        <v>29</v>
       </c>
       <c r="D17">
-        <v>12.9</v>
+        <v>29</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2292,10 +2295,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>28.3</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>28.3</v>
+        <v>30</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2312,16 +2315,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>13.4</v>
+        <v>33</v>
       </c>
       <c r="D19">
-        <v>13.5</v>
+        <v>33</v>
       </c>
       <c r="E19">
-        <v>0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.7462686567164152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2332,16 +2335,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>28.6</v>
+        <v>30</v>
       </c>
       <c r="D20">
-        <v>28.5</v>
+        <v>30</v>
       </c>
       <c r="E20">
-        <v>-0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>-0.3496503496503546</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2352,12 +2355,15 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -2369,10 +2375,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1.6</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>1.6</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2389,10 +2395,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>7</v>
       </c>
       <c r="D23">
-        <v>0.4</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2409,12 +2415,15 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -2426,10 +2435,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>5.6</v>
+        <v>18</v>
       </c>
       <c r="D25">
-        <v>5.6</v>
+        <v>18</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2446,16 +2455,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>17.7</v>
+        <v>22</v>
       </c>
       <c r="D26">
-        <v>17.8</v>
+        <v>22</v>
       </c>
       <c r="E26">
-        <v>0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0.5649717514124375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2466,10 +2475,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>5.2</v>
+        <v>21</v>
       </c>
       <c r="D27">
-        <v>5.2</v>
+        <v>21</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -2486,10 +2495,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>17.7</v>
+        <v>22</v>
       </c>
       <c r="D28">
-        <v>17.7</v>
+        <v>22</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2615,16 +2624,16 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>2.48</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>-0.02000000000000002</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>-0.8000000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2635,16 +2644,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>7.8</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>7.89</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.08999999999999986</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1.153846153846152</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2655,16 +2664,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>8.1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-0.0600000000000005</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-0.7407407407407469</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2743,16 +2752,16 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>10.6</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>10.59</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>-0.009999999999999787</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>-0.09433962264150743</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2763,16 +2772,16 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>26.04</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.03999999999999915</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.1538461538461506</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2783,16 +2792,16 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>11.6</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>11.57</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>-0.02999999999999936</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>-0.2586206896551669</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2803,16 +2812,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>26.3</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>26.4</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.09999999999999787</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.3802281368821211</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2840,10 +2849,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2860,16 +2869,16 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0.14</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>40.00000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2897,16 +2906,16 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>12.9</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>12.94</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.03999999999999915</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>0.3100775193798383</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2917,16 +2926,16 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>28.3</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>28.26</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>-0.03999999999999915</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>-0.1413427561837426</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2937,16 +2946,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>13.4</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>13.45</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.04999999999999893</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.373134328358201</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2957,16 +2966,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>28.6</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>28.46</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>-0.1400000000000006</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>-0.4895104895104915</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2977,16 +2986,16 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
+        <v>0.03</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2997,16 +3006,16 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>1.58</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>-0.02000000000000002</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>-1.250000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3017,16 +3026,16 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0.35</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>-0.05000000000000004</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>-12.50000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3037,16 +3046,16 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
+        <v>0.03</v>
+      </c>
+      <c r="F24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3057,16 +3066,16 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>5.61</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.01000000000000068</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.1785714285714406</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3077,16 +3086,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>17.8</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.5649717514124375</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3097,16 +3106,16 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>5.2</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>5.23</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>0.03000000000000025</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>0.5769230769230818</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3117,16 +3126,16 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>17.75</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>0.05000000000000071</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>0.2824858757062187</v>
       </c>
     </row>
     <row r="29" spans="1:6">

</xml_diff>